<commit_message>
second wave of analysis
</commit_message>
<xml_diff>
--- a/SC_poff.xlsx
+++ b/SC_poff.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Decade\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\Data_analysis\NBA_player_Decde\Data_nab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BC196F-EAED-4328-9545-46F85D21237D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8DE2A242-E464-4B7B-BD6A-23D251CB8F0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -324,14 +323,14 @@
     <t>L (-9)</t>
   </si>
   <si>
-    <t>2006 Playoffs</t>
+    <t>Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -687,16 +686,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FAAC69-A04A-474B-A3EE-B5EA91E93E42}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,7 +784,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -880,7 +879,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -972,7 +971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1064,7 +1063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1156,7 +1155,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1248,7 +1247,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1340,7 +1339,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1435,7 +1434,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1530,7 +1529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1622,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1714,7 +1713,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1806,7 +1805,7 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1895,7 +1894,7 @@
         <v>-19</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1987,7 +1986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2082,7 +2081,7 @@
         <v>-27</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2174,7 +2173,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2266,7 +2265,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2361,7 +2360,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2453,7 +2452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2548,7 +2547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2640,7 +2639,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2732,7 +2731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2827,7 +2826,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2922,7 +2921,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3014,7 +3013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3106,7 +3105,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3201,7 +3200,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3296,7 +3295,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3385,7 +3384,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3480,7 +3479,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3572,7 +3571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -3664,7 +3663,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="33" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -3759,7 +3758,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3854,7 +3853,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="35" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3946,7 +3945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -4038,7 +4037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -4130,7 +4129,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="38" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -4222,7 +4221,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="39" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -4317,7 +4316,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -4409,7 +4408,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -4504,7 +4503,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -4596,7 +4595,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -4685,7 +4684,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -4777,7 +4776,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -4872,7 +4871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -4961,7 +4960,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -5050,7 +5049,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -5139,7 +5138,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -5231,7 +5230,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -5326,7 +5325,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -5418,7 +5417,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -5510,7 +5509,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="53" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -5602,7 +5601,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -5697,7 +5696,7 @@
         <v>-39</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -5792,7 +5791,7 @@
         <v>-19</v>
       </c>
     </row>
-    <row r="56" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -5884,7 +5883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -5979,7 +5978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:31">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -6071,7 +6070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -6160,7 +6159,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:31">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -6249,7 +6248,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:31">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -6344,7 +6343,7 @@
         <v>-22</v>
       </c>
     </row>
-    <row r="62" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:31">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -6439,7 +6438,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:31">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -6531,7 +6530,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="64" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:31">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -6626,7 +6625,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="65" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:31">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -6718,7 +6717,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="66" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:31">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -6810,7 +6809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:31">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -6902,7 +6901,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:31">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -6997,7 +6996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:31">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -7092,7 +7091,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:31">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -7184,7 +7183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:31">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -7276,7 +7275,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:31">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -7371,7 +7370,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:31">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -7466,7 +7465,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:31">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -7558,7 +7557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:31">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -7650,7 +7649,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:31">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -7745,7 +7744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:31">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -7840,7 +7839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:31">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -7929,7 +7928,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:31">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -8021,7 +8020,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:31">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -8116,7 +8115,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:31">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -8211,7 +8210,7 @@
         <v>-26</v>
       </c>
     </row>
-    <row r="82" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:31">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -8303,7 +8302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:31">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -8392,7 +8391,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="84" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:31">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -8481,7 +8480,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:31">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -8573,7 +8572,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="86" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:31">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -8665,7 +8664,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:31">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -8754,7 +8753,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:31">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -8843,7 +8842,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="89" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:31">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -8935,7 +8934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:31">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -9030,7 +9029,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="91" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:31">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -9125,7 +9124,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:31">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -9217,7 +9216,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:31">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -9312,7 +9311,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:31">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -9407,7 +9406,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="95" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:31">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -9499,7 +9498,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:31">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -9591,7 +9590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:31">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -9686,7 +9685,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="98" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:31">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -9775,7 +9774,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:31">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -9867,7 +9866,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:31">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -9959,7 +9958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:31">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -10051,7 +10050,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:31">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -10146,7 +10145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:31">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -10241,7 +10240,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:31">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -10333,7 +10332,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:31">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -10425,7 +10424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:31">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -10520,7 +10519,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:31">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -10615,7 +10614,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="108" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:31">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -10707,7 +10706,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="109" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:31">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -10802,7 +10801,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="110" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:31">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -10894,7 +10893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:31">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -10986,7 +10985,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:31">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -11081,7 +11080,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="113" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:31">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -11176,7 +11175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:31">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -11268,7 +11267,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:31">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -11363,7 +11362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:31">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -11455,7 +11454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:31">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -11547,7 +11546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:31">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -11642,7 +11641,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="119" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:31">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -11737,7 +11736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:31">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -11832,7 +11831,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="121" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:31">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -11927,7 +11926,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:31">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -12019,7 +12018,7 @@
         <v>-8</v>
       </c>
     </row>
-    <row r="123" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:31">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -12111,7 +12110,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="124" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:31">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -12206,7 +12205,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="125" spans="1:31" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:31">
       <c r="A125" s="1">
         <v>124</v>
       </c>

</xml_diff>